<commit_message>
ventura reservas e ical
</commit_message>
<xml_diff>
--- a/storage/app/utils/Categories.xlsx
+++ b/storage/app/utils/Categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\Escritorio\boots\bootsPeru\storage\app\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\Escritorio\ventura\ventura\storage\app\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D1F7D8-FB27-459F-BF0A-02C6B848D770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF46C07E-F0A5-4B11-8687-5E3C339EFDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Id</t>
   </si>
@@ -33,10 +33,7 @@
     <t>Categorias</t>
   </si>
   <si>
-    <t>Autoradios</t>
-  </si>
-  <si>
-    <t>Accesorios</t>
+    <t>Departamentos</t>
   </si>
 </sst>
 </file>
@@ -437,7 +434,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,15 +467,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>

</xml_diff>